<commit_message>
flow calcs for all scenarios and their precentages
</commit_message>
<xml_diff>
--- a/calculated_Flows.xlsx
+++ b/calculated_Flows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsaberi\GitHub\Unsat-Sat-Flow-Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4010D81F-AE37-48F4-A20A-68ECE060648D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5275C3F2-2C65-4EC7-AF64-62B9B5FD995C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calculated_Flows" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Flow Type</t>
   </si>
@@ -56,15 +56,9 @@
     <t>POND</t>
   </si>
   <si>
-    <t>sce1 (MF-NWT)</t>
-  </si>
-  <si>
     <t>DNS1</t>
   </si>
   <si>
-    <t>sce2 (MF-NWT)</t>
-  </si>
-  <si>
     <t>DNS2</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>Downgradient WT (ft) (above bottom of the ash pond)</t>
   </si>
   <si>
-    <t>Scenario 0</t>
-  </si>
-  <si>
     <t>Scenario 1</t>
   </si>
   <si>
@@ -152,16 +143,34 @@
     <t>sce2 - MFNWT</t>
   </si>
   <si>
-    <t>sce0 - MFNWT</t>
-  </si>
-  <si>
-    <t>Sce0</t>
-  </si>
-  <si>
     <t>MF-NWT Refined Simulation Results</t>
   </si>
   <si>
     <t>MF6 Refined Simulation Results</t>
+  </si>
+  <si>
+    <t>sce3 - MFNWT</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>sce1 (MF-NWT Refined)</t>
+  </si>
+  <si>
+    <t>sce2 (MF-NWT Refined)</t>
+  </si>
+  <si>
+    <t>sce1 (MF6 Refined)</t>
+  </si>
+  <si>
+    <t>sce2 (MF6 Refined)</t>
+  </si>
+  <si>
+    <t>sce1 (MF-NWT 3-Layer)</t>
+  </si>
+  <si>
+    <t>sce2 (MF-NWT 3-Layer)</t>
   </si>
 </sst>
 </file>
@@ -877,7 +886,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -954,6 +963,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1310,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,20 +1381,20 @@
         <v>122.18992366333001</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G2" s="18">
-        <f>C2/C5</f>
-        <v>4.4493369426213132E-2</v>
+        <f>K21/L21</f>
+        <v>0.13610819295018456</v>
       </c>
       <c r="H2" s="18">
-        <f>C2/C8</f>
-        <v>4.4481172678949459E-2</v>
+        <f>K21/M21</f>
+        <v>0.13598408289109923</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>15298.8131466796</v>
@@ -1396,20 +1406,20 @@
         <v>14727.141821875</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="G3" s="18">
-        <f>D2/D5</f>
-        <v>5.0703649322880037E-3</v>
+        <f>K22/L22</f>
+        <v>2.0364359028360361E-2</v>
       </c>
       <c r="H3" s="18">
-        <f>D2/D8</f>
-        <v>5.0688487495434151E-3</v>
+        <f>K22/M22</f>
+        <v>2.0361717470228545E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>9732.7290629882791</v>
@@ -1421,20 +1431,20 @@
         <v>9371.7002329101506</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="18">
-        <f>E13/F13</f>
+        <f>H21/I21</f>
         <v>0.19662456014268279</v>
       </c>
       <c r="H4" s="18">
-        <f>E13/G13</f>
+        <f>H21/J21</f>
         <v>0.20280565510414061</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="11">
         <f>B3+B4</f>
@@ -1449,20 +1459,20 @@
         <v>24098.842054785149</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="18">
-        <f>E14/F14</f>
+        <f>H22/I22</f>
         <v>4.4135320791387926E-2</v>
       </c>
       <c r="H5" s="18">
-        <f>E14/G14</f>
+        <f>H22/J22</f>
         <v>4.6571352790534905E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>17904.231821288999</v>
@@ -1473,10 +1483,21 @@
       <c r="D6">
         <v>17249.101636914002</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="18">
+        <f>N21/O21</f>
+        <v>0.13490353039872899</v>
+      </c>
+      <c r="H6" s="18">
+        <f>N21/P21</f>
+        <v>0.13924259767460187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>7117.8664141113204</v>
@@ -1487,10 +1508,21 @@
       <c r="D7">
         <v>6856.9488098144502</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="18">
+        <f>N22/O22</f>
+        <v>2.0181293518814713E-2</v>
+      </c>
+      <c r="H7" s="18">
+        <f>N22/P22</f>
+        <v>2.0609945026323129E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="11">
         <f>B6+B7</f>
@@ -1504,13 +1536,35 @@
         <f>D6+D7</f>
         <v>24106.050446728452</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="18">
+        <f>E21/F21</f>
+        <v>4.4493369426213132E-2</v>
+      </c>
+      <c r="H8" s="18">
+        <f>E21/G21</f>
+        <v>4.4481172678949459E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
+      <c r="F9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="18">
+        <f>E22/F22</f>
+        <v>5.0703649322880037E-3</v>
+      </c>
+      <c r="H9" s="18">
+        <f>E22/G22</f>
+        <v>5.0688487495434151E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
@@ -1524,25 +1578,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="E12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1550,7 +1604,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2">
         <v>0.145682035857325</v>
@@ -1579,7 +1633,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>0.140662279596486</v>
@@ -1608,7 +1662,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2">
         <v>0.15159707609300699</v>
@@ -1653,284 +1707,275 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E18" s="31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
       <c r="H18" s="32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="31" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L18" s="31"/>
       <c r="M18" s="31"/>
       <c r="N18" s="31" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>23</v>
-      </c>
       <c r="H19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="K19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>23</v>
-      </c>
       <c r="N19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P19" s="22" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="26">
+      <c r="E20" s="34"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="26">
         <f>C2</f>
         <v>1076.5682381957999</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F21" s="27">
         <f>C5</f>
         <v>24196.149945019519</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G21" s="27">
         <f>C8</f>
         <v>24202.78453461911</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H21" s="28">
         <f>E13*2</f>
         <v>5105.400316234508</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I21" s="28">
         <f>F13*2</f>
         <v>25965.221804080415</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J21" s="28">
         <f>G13*2</f>
         <v>25173.855796145759</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K21" s="26">
         <v>3277.88</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L21" s="27">
         <v>24082.9</v>
       </c>
-      <c r="M20" s="27">
+      <c r="M21" s="27">
         <v>24104.880000000001</v>
       </c>
-      <c r="N20" s="26">
+      <c r="N21" s="26">
         <v>3286.88</v>
       </c>
-      <c r="O20" s="27">
+      <c r="O21" s="27">
         <v>24364.67</v>
       </c>
-      <c r="P20" s="27">
+      <c r="P21" s="27">
         <v>23605.42</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D21" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="29">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D22" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="29">
         <f>D2</f>
         <v>122.18992366333001</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F22" s="30">
         <f>D5</f>
         <v>24098.842054785149</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G22" s="30">
         <f>D8</f>
         <v>24106.050446728452</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H22" s="28">
         <f>E14*2</f>
         <v>1131.9838814722423</v>
       </c>
-      <c r="I21" s="28">
-        <f t="shared" ref="I21:J22" si="0">F14*2</f>
+      <c r="I22" s="28">
+        <f t="shared" ref="I22:J22" si="0">F14*2</f>
         <v>25648.026595812691</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J22" s="28">
         <f t="shared" si="0"/>
         <v>24306.441914272782</v>
       </c>
-      <c r="K21" s="29">
+      <c r="K22" s="29">
         <v>488.5</v>
       </c>
-      <c r="L21" s="30">
+      <c r="L22" s="30">
         <v>23987.988000000001</v>
       </c>
-      <c r="M21" s="30">
+      <c r="M22" s="30">
         <v>23991.1</v>
       </c>
-      <c r="N21" s="29">
+      <c r="N22" s="29">
         <v>487.04</v>
       </c>
-      <c r="O21" s="30">
+      <c r="O22" s="30">
         <v>24133.24</v>
       </c>
-      <c r="P21" s="30">
+      <c r="P22" s="30">
         <v>23631.31</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="28">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="28">
         <f>B2</f>
         <v>7921.63689824218</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F23" s="28">
         <f>B5</f>
         <v>25031.542209667881</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G23" s="28">
         <f>B8</f>
         <v>25022.098235400321</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H23" s="28">
         <f>E15*2</f>
         <v>9013.0202057420811</v>
       </c>
-      <c r="I22" s="28">
-        <f t="shared" si="0"/>
+      <c r="I23" s="28">
+        <f>F15*2</f>
         <v>26929.73193921458</v>
       </c>
-      <c r="J22" s="28">
-        <f t="shared" si="0"/>
+      <c r="J23" s="28">
+        <f>G15*2</f>
         <v>26195.974748871609</v>
       </c>
-      <c r="K22" s="28">
+      <c r="K23" s="28">
         <v>8021.1</v>
       </c>
-      <c r="L22" s="28">
+      <c r="L23" s="28">
         <v>24935.99</v>
       </c>
-      <c r="M22" s="28">
+      <c r="M23" s="28">
         <v>24973.279999999999</v>
       </c>
-      <c r="N22" s="28">
+      <c r="N23" s="28">
         <v>7975.16</v>
       </c>
-      <c r="O22" s="28">
+      <c r="O23" s="28">
         <v>25177.85</v>
       </c>
-      <c r="P22" s="28">
+      <c r="P23" s="28">
         <v>24602.89</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="F26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="G26" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="7">
-        <v>2.83</v>
-      </c>
-      <c r="C26" s="7">
-        <v>2.83</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="F26" s="21">
-        <v>62</v>
-      </c>
-      <c r="G26" s="21">
-        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B27" s="7">
         <v>2.83</v>
       </c>
-      <c r="C27" s="14">
-        <v>0.28299999999999997</v>
+      <c r="C27" s="7">
+        <v>2.83</v>
       </c>
       <c r="D27" s="7">
-        <v>0.42</v>
+        <v>0.2</v>
       </c>
       <c r="E27" s="7">
         <v>0.2</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="21">
         <v>62</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="21">
         <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B28" s="7">
         <v>2.83</v>
       </c>
-      <c r="C28" s="15">
-        <v>2.8299999999999999E-2</v>
+      <c r="C28" s="14">
+        <v>0.28299999999999997</v>
       </c>
       <c r="D28" s="7">
         <v>0.42</v>
@@ -1945,9 +1990,32 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C29" s="10" t="s">
-        <v>34</v>
+    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2.83</v>
+      </c>
+      <c r="C29" s="15">
+        <v>2.8299999999999999E-2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F29" s="7">
+        <v>62</v>
+      </c>
+      <c r="G29" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C30" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>